<commit_message>
add use case for import deadline
</commit_message>
<xml_diff>
--- a/Database_Excel/DS_DiemCourse.xlsx
+++ b/Database_Excel/DS_DiemCourse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\MyDocuments\Subject\Nhap Mon Cong Nghe Phan Mem\GitHub\Database_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ideapad\Documents\GitHub\intro2se-cq21_3-group10\Database_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10D286A-B5CE-42FC-8542-1DC36624E08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F0CAC2-365C-4D69-AEED-FCED87884A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3398F598-547C-4491-8B65-D98C51B87428}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3398F598-547C-4491-8B65-D98C51B87428}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>StudentID</t>
+    <t>user_id</t>
   </si>
   <si>
-    <t>Score</t>
+    <t>score</t>
   </si>
 </sst>
 </file>
@@ -106,9 +106,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -146,7 +146,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -252,7 +252,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,12 +405,12 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -426,7 +426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>1+A2</f>
         <v>5</v>
@@ -435,79 +435,79 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A28" si="0">1+A3</f>
         <v>6</v>
       </c>
       <c r="B4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="B5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B9">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -516,52 +516,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B13">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B17">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -570,52 +570,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B19">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B20">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B23">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -624,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -633,7 +633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -642,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <f>1+A26</f>
         <v>29</v>
@@ -651,7 +651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>30</v>

</xml_diff>